<commit_message>
Weekly reports and Timesheets
Weekly reports and weekly timesheets. Made some dates corrections on
some  weekly Timesheets
</commit_message>
<xml_diff>
--- a/Documents/Finance/Timesheets/Paul Mathema/SWENG timesheet week 5.xlsx
+++ b/Documents/Finance/Timesheets/Paul Mathema/SWENG timesheet week 5.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PM\Documents\GitHub\SWENG\Documents\Finance\Timesheets\Paul Mathema\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="600" windowWidth="20740" windowHeight="11760"/>
+    <workbookView xWindow="645" yWindow="600" windowWidth="20745" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="valuevx">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -588,54 +593,54 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -944,106 +949,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="12" customWidth="1"/>
     <col min="2" max="8" width="9" style="12" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" style="12" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="12" customWidth="1"/>
     <col min="10" max="10" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="14" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-    </row>
-    <row r="2" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="1" spans="1:9" s="14" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+    </row>
+    <row r="2" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-    </row>
-    <row r="4" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A4" s="30"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="31" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+    </row>
+    <row r="4" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="32" t="s">
+      <c r="F4" s="34"/>
+      <c r="G4" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-    </row>
-    <row r="5" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="30"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+    </row>
+    <row r="5" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="G5" s="9"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="31" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="32" t="s">
+      <c r="F6" s="34"/>
+      <c r="G6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-    </row>
-    <row r="7" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A7" s="35" t="s">
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+    </row>
+    <row r="7" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="31" t="s">
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="29"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="36">
         <v>41673</v>
       </c>
@@ -1052,11 +1057,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="9" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" ht="27" customHeight="1">
+    <row r="10" spans="1:9" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>5</v>
       </c>
@@ -1085,7 +1090,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="11" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <f>G8</f>
         <v>41673</v>
@@ -1104,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="12" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24">
         <f t="shared" ref="A12:A17" si="1">A11+1</f>
         <v>41674</v>
@@ -1123,7 +1128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="13" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24">
         <f t="shared" si="1"/>
         <v>41675</v>
@@ -1142,7 +1147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="14" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24">
         <f t="shared" si="1"/>
         <v>41676</v>
@@ -1161,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="15" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
         <f t="shared" si="1"/>
         <v>41677</v>
@@ -1180,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="16" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24">
         <f t="shared" si="1"/>
         <v>41678</v>
@@ -1197,7 +1202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="17" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24">
         <f t="shared" si="1"/>
         <v>41679</v>
@@ -1216,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="18" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>14</v>
       </c>
@@ -1252,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="19" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>15</v>
       </c>
@@ -1281,7 +1286,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="20" spans="1:9" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -1318,85 +1323,100 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1"/>
-    <row r="22" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="13">
         <f>I18</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
+    <row r="23" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="13">
         <f>I20</f>
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1"/>
-    <row r="25" spans="1:9" s="12" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A25" s="32" t="s">
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:9" s="12" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="43">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="32">
         <v>41679</v>
       </c>
-      <c r="E25" s="33"/>
-    </row>
-    <row r="26" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A26" s="39" t="s">
+      <c r="E25" s="31"/>
+    </row>
+    <row r="26" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="39" t="s">
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="40"/>
-    </row>
-    <row r="27" spans="1:9" s="12" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A27" s="32" t="s">
+      <c r="E26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" s="12" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="43">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="32">
         <v>41682</v>
       </c>
-      <c r="E27" s="33"/>
-    </row>
-    <row r="28" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1">
-      <c r="A28" s="39" t="s">
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="39" t="s">
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="40"/>
-    </row>
-    <row r="29" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1"/>
-    <row r="30" spans="1:9" ht="12">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
+      <c r="E28" s="27"/>
+    </row>
+    <row r="29" spans="1:9" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="A30:C30"/>
@@ -1407,21 +1427,6 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>